<commit_message>
Updated budget, progress report and workplan
</commit_message>
<xml_diff>
--- a/doc/Budget.xlsx
+++ b/doc/Budget.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GuilleX7\Documents\GitHub\Acme-Planner\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{311079F5-9CA6-4FB7-A247-EDF6D5E46134}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902B7B5D-1EFB-49B2-94A2-0F09A8BFFEDB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E6FE04B6-807F-41B9-BCEE-B9B32721F2E1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Budget</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t>Total hours:</t>
+  </si>
+  <si>
+    <t>Total estimated hours:</t>
+  </si>
+  <si>
+    <t>Total work hours</t>
   </si>
 </sst>
 </file>
@@ -665,7 +671,7 @@
   <dimension ref="B1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,6 +681,7 @@
     <col min="3" max="3" width="22.7109375" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
     <col min="5" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="9" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1023,7 +1030,7 @@
         <v>17.5</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F16" s="21">
         <f>SUM(F12:F15)</f>
@@ -1044,9 +1051,13 @@
     <row r="17" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>24</v>
+      </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -1058,9 +1069,14 @@
     <row r="18" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="17">
+        <v>11.7</v>
+      </c>
+      <c r="G18" s="13">
+        <f>D12*F18</f>
+        <v>292.5</v>
+      </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -1072,9 +1088,14 @@
     <row r="19" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="17">
+        <v>12.28</v>
+      </c>
+      <c r="G19" s="13">
+        <f>D13*F19</f>
+        <v>184.2</v>
+      </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -1086,9 +1107,14 @@
     <row r="20" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="17">
+        <v>14.65</v>
+      </c>
+      <c r="G20" s="13">
+        <f>D14*F20</f>
+        <v>219.75</v>
+      </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -1100,9 +1126,14 @@
     <row r="21" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="17">
+        <v>11.93</v>
+      </c>
+      <c r="G21" s="13">
+        <f>D15*F21</f>
+        <v>178.95</v>
+      </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -1114,9 +1145,17 @@
     <row r="22" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
+      <c r="E22" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="21">
+        <f>SUM(F18:F21)</f>
+        <v>50.559999999999995</v>
+      </c>
+      <c r="G22" s="20">
+        <f>SUM(G18:G21)</f>
+        <v>875.40000000000009</v>
+      </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>

</xml_diff>

<commit_message>
Applied all the fixed for the deliverable
</commit_message>
<xml_diff>
--- a/doc/Budget.xlsx
+++ b/doc/Budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GuilleX7\Documents\GitHub\Acme-Planner\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902B7B5D-1EFB-49B2-94A2-0F09A8BFFEDB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C12A326-B4C7-4E6E-9FF0-23B2114BAF59}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E6FE04B6-807F-41B9-BCEE-B9B32721F2E1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Budget</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>Total work hours</t>
+  </si>
+  <si>
+    <t>Total cost</t>
   </si>
 </sst>
 </file>
@@ -671,7 +674,7 @@
   <dimension ref="B1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1056,7 +1059,7 @@
         <v>28</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>

</xml_diff>

<commit_message>
Added analyst time for the budget
</commit_message>
<xml_diff>
--- a/doc/Budget.xlsx
+++ b/doc/Budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GuilleX7\Documents\GitHub\Acme-Planner\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C12A326-B4C7-4E6E-9FF0-23B2114BAF59}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E97726BE-BA1B-4654-B39C-66A60E1E126F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E6FE04B6-807F-41B9-BCEE-B9B32721F2E1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="31">
   <si>
     <t>Budget</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>Total cost</t>
+  </si>
+  <si>
+    <t>Analyst</t>
   </si>
 </sst>
 </file>
@@ -295,7 +298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -357,6 +360,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -671,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF81983B-6797-4DAB-9661-559EA0F2B9F0}">
-  <dimension ref="B1:N26"/>
+  <dimension ref="B1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,18 +959,18 @@
         <v>17</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="D13" s="13">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="17">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="G13" s="13">
         <f>D13*F13</f>
-        <v>375</v>
+        <v>50</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -973,7 +982,7 @@
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>21</v>
@@ -999,21 +1008,21 @@
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="D15" s="13">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="17">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="G15" s="13">
         <f>D15*F15</f>
-        <v>375</v>
+        <v>50</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -1024,24 +1033,22 @@
       <c r="N15" s="1"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="18"/>
-      <c r="C16" s="19" t="s">
+      <c r="B16" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="13">
+        <v>15</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="17">
         <v>25</v>
       </c>
-      <c r="D16" s="20">
-        <f>AVERAGE(D12:D15)</f>
-        <v>17.5</v>
-      </c>
-      <c r="E16" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" s="21">
-        <f>SUM(F12:F15)</f>
-        <v>100</v>
-      </c>
-      <c r="G16" s="20">
-        <f>SUM(G12:G15)</f>
-        <v>1750</v>
+      <c r="G16" s="13">
+        <f>D16*F16</f>
+        <v>375</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -1051,15 +1058,23 @@
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
     </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="G17" s="16" t="s">
-        <v>29</v>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="13">
+        <v>25</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="17">
+        <v>2</v>
+      </c>
+      <c r="G17" s="13">
+        <f>D17*F17</f>
+        <v>50</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -1069,16 +1084,23 @@
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
     </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="13">
+        <v>15</v>
+      </c>
       <c r="E18" s="2"/>
       <c r="F18" s="17">
-        <v>11.7</v>
+        <v>25</v>
       </c>
       <c r="G18" s="13">
-        <f>D12*F18</f>
-        <v>292.5</v>
+        <f>D18*F18</f>
+        <v>375</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -1088,16 +1110,25 @@
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
     </row>
-    <row r="19" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="17">
-        <v>12.28</v>
-      </c>
-      <c r="G19" s="13">
-        <f>D13*F19</f>
-        <v>184.2</v>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B19" s="18"/>
+      <c r="C19" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="20">
+        <f>AVERAGE(D12:D17)</f>
+        <v>21.666666666666668</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="21">
+        <f>SUM(F12:F17)</f>
+        <v>81</v>
+      </c>
+      <c r="G19" s="20">
+        <f>SUM(G12:G17)</f>
+        <v>1525</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -1107,16 +1138,22 @@
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
     </row>
-    <row r="20" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="17">
-        <v>14.65</v>
-      </c>
-      <c r="G20" s="13">
-        <f>D14*F20</f>
-        <v>219.75</v>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B20" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="22"/>
+      <c r="F20" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -1126,16 +1163,23 @@
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
     </row>
-    <row r="21" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B21" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="13">
+        <v>25</v>
+      </c>
       <c r="E21" s="2"/>
-      <c r="F21" s="17">
-        <v>11.93</v>
+      <c r="F21" s="23">
+        <v>11.7</v>
       </c>
       <c r="G21" s="13">
-        <f>D15*F21</f>
-        <v>178.95</v>
+        <f>D12*F21</f>
+        <v>292.5</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -1145,19 +1189,23 @@
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
     </row>
-    <row r="22" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="F22" s="21">
-        <f>SUM(F18:F21)</f>
-        <v>50.559999999999995</v>
-      </c>
-      <c r="G22" s="20">
-        <f>SUM(G18:G21)</f>
-        <v>875.40000000000009</v>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B22" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="13">
+        <v>25</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="24">
+        <v>3</v>
+      </c>
+      <c r="G22" s="13">
+        <f t="shared" ref="G22:G27" si="4">D13*F22</f>
+        <v>75</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -1167,12 +1215,24 @@
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
     </row>
-    <row r="23" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B23" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="13">
+        <v>15</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="23">
+        <v>12.28</v>
+      </c>
+      <c r="G23" s="13">
+        <f t="shared" si="4"/>
+        <v>184.2</v>
+      </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -1181,12 +1241,24 @@
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
     </row>
-    <row r="24" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B24" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="13">
+        <v>25</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="24">
+        <v>3</v>
+      </c>
+      <c r="G24" s="13">
+        <f t="shared" si="4"/>
+        <v>75</v>
+      </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -1195,12 +1267,24 @@
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
     </row>
-    <row r="25" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B25" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="13">
+        <v>15</v>
+      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" s="23">
+        <v>14.65</v>
+      </c>
+      <c r="G25" s="13">
+        <f t="shared" si="4"/>
+        <v>219.75</v>
+      </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -1209,12 +1293,24 @@
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
     </row>
-    <row r="26" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B26" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="13">
+        <v>25</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="24">
+        <v>3</v>
+      </c>
+      <c r="G26" s="13">
+        <f t="shared" si="4"/>
+        <v>75</v>
+      </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -1223,6 +1319,46 @@
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
     </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B27" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="13">
+        <v>15</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="23">
+        <v>11.93</v>
+      </c>
+      <c r="G27" s="13">
+        <f t="shared" si="4"/>
+        <v>178.95</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B28" s="18"/>
+      <c r="C28" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="20">
+        <f>AVERAGE(D21:D26)</f>
+        <v>21.666666666666668</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" s="21">
+        <f>SUM(F21:F27)</f>
+        <v>59.559999999999995</v>
+      </c>
+      <c r="G28" s="20">
+        <f>SUM(G21:G27)</f>
+        <v>1100.4000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>